<commit_message>
Save Excel Content Data to DB DONE
</commit_message>
<xml_diff>
--- a/uploads/Rekap Case Trx 2021.xlsx
+++ b/uploads/Rekap Case Trx 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bleizing/Bleizing/Kerja/BRI/DOCS/Rekap Case Docs/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2E11FD-9105-8F4E-B216-F5DFC7337650}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF71690-0475-6E4A-8689-10229CC9E286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="500" windowWidth="28700" windowHeight="12540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="500" windowWidth="28700" windowHeight="12540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JAN 2021" sheetId="1" r:id="rId1"/>
@@ -4368,10 +4368,6 @@
     <t>Ekskalasi ke tim CAO</t>
   </si>
   <si>
-    <t>sempat terjadi response code 91 naik, dari other bank dgn kode bank 013 (Bank Permata). Transaksi Bank Permata Timeout, Transaksi ke Nomer Tujuan Virtual Account,, 
-dengan Prefix 896502XXXXX,,  855609XXXXX  dan 856666XXXXX</t>
-  </si>
-  <si>
     <t>03:34 WIB</t>
   </si>
   <si>
@@ -4984,6 +4980,9 @@
   </si>
   <si>
     <t>16:42 WIB</t>
+  </si>
+  <si>
+    <t>sempat terjadi response code 91 naik, dari other bank dgn kode bank 013 (Bank Permata). Transaksi Bank Permata Timeout, Transaksi ke Nomer Tujuan Virtual Account, dengan Prefix 896502XXXXX,  855609XXXXX  dan 856666XXXXX</t>
   </si>
 </sst>
 </file>
@@ -35618,7 +35617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A288" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A292" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D300" sqref="D300"/>
     </sheetView>
   </sheetViews>
@@ -39450,7 +39449,7 @@
         <v>44258</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>783</v>
@@ -39462,7 +39461,7 @@
         <v>14</v>
       </c>
       <c r="G108" s="7" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="H108" s="6" t="s">
         <v>29</v>
@@ -39666,7 +39665,7 @@
         <v>277</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="E114" s="6" t="s">
         <v>38</v>
@@ -39702,7 +39701,7 @@
         <v>1065</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>80</v>
@@ -39711,7 +39710,7 @@
         <v>14</v>
       </c>
       <c r="G115" s="11" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="H115" s="6" t="s">
         <v>70</v>
@@ -39807,7 +39806,7 @@
         <v>44259</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>178</v>
@@ -39855,7 +39854,7 @@
         <v>14</v>
       </c>
       <c r="G119" s="11" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="H119" s="6" t="s">
         <v>1361</v>
@@ -39891,7 +39890,7 @@
         <v>14</v>
       </c>
       <c r="G120" s="7" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="H120" s="6" t="s">
         <v>1361</v>
@@ -39927,7 +39926,7 @@
         <v>14</v>
       </c>
       <c r="G121" s="7" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="H121" s="6" t="s">
         <v>1361</v>
@@ -39963,7 +39962,7 @@
         <v>14</v>
       </c>
       <c r="G122" s="7" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="H122" s="6" t="s">
         <v>1361</v>
@@ -39999,7 +39998,7 @@
         <v>14</v>
       </c>
       <c r="G123" s="7" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="H123" s="6" t="s">
         <v>1361</v>
@@ -40023,10 +40022,10 @@
         <v>44259</v>
       </c>
       <c r="C124" s="6" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D124" s="6" t="s">
         <v>1462</v>
-      </c>
-      <c r="D124" s="6" t="s">
-        <v>1463</v>
       </c>
       <c r="E124" s="6" t="s">
         <v>130</v>
@@ -40035,7 +40034,7 @@
         <v>14</v>
       </c>
       <c r="G124" s="7" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="H124" s="6" t="s">
         <v>1361</v>
@@ -40062,7 +40061,7 @@
         <v>160</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="E125" s="6" t="s">
         <v>80</v>
@@ -40095,7 +40094,7 @@
         <v>44259</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>1367</v>
@@ -40131,7 +40130,7 @@
         <v>44259</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>1002</v>
@@ -40143,7 +40142,7 @@
         <v>14</v>
       </c>
       <c r="G127" s="7" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="H127" s="6" t="s">
         <v>1361</v>
@@ -40170,7 +40169,7 @@
         <v>287</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="E128" s="6" t="s">
         <v>44</v>
@@ -40242,7 +40241,7 @@
         <v>1431</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>13</v>
@@ -40251,7 +40250,7 @@
         <v>14</v>
       </c>
       <c r="G130" s="7" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="H130" s="6" t="s">
         <v>1361</v>
@@ -40286,7 +40285,7 @@
         <v>14</v>
       </c>
       <c r="G131" s="7" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="H131" s="6" t="s">
         <v>1361</v>
@@ -40347,7 +40346,7 @@
         <v>914</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="E133" s="6" t="s">
         <v>90</v>
@@ -40356,7 +40355,7 @@
         <v>14</v>
       </c>
       <c r="G133" s="7" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="H133" s="6" t="s">
         <v>1361</v>
@@ -40382,7 +40381,7 @@
         <v>721</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="E134" s="6" t="s">
         <v>80</v>
@@ -40414,7 +40413,7 @@
         <v>44259</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="D135" s="6" t="s">
         <v>532</v>
@@ -40487,7 +40486,7 @@
         <v>288</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="E137" s="6" t="s">
         <v>80</v>
@@ -40519,10 +40518,10 @@
         <v>44259</v>
       </c>
       <c r="C138" s="6" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D138" s="6" t="s">
         <v>1480</v>
-      </c>
-      <c r="D138" s="6" t="s">
-        <v>1481</v>
       </c>
       <c r="E138" s="6" t="s">
         <v>27</v>
@@ -40595,13 +40594,13 @@
         <v>126</v>
       </c>
       <c r="E140" s="6" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F140" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G140" s="7" t="s">
         <v>1486</v>
-      </c>
-      <c r="F140" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G140" s="7" t="s">
-        <v>1487</v>
       </c>
       <c r="H140" s="6" t="s">
         <v>1361</v>
@@ -40636,7 +40635,7 @@
         <v>14</v>
       </c>
       <c r="G141" s="7" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="H141" s="6" t="s">
         <v>29</v>
@@ -40659,13 +40658,13 @@
         <v>44260</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="D142" s="6" t="s">
         <v>338</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="F142" s="6" t="s">
         <v>14</v>
@@ -40694,10 +40693,10 @@
         <v>44260</v>
       </c>
       <c r="C143" s="6" t="s">
+        <v>1497</v>
+      </c>
+      <c r="D143" s="6" t="s">
         <v>1498</v>
-      </c>
-      <c r="D143" s="6" t="s">
-        <v>1499</v>
       </c>
       <c r="E143" s="6" t="s">
         <v>27</v>
@@ -40729,10 +40728,10 @@
         <v>44260</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="E144" s="6" t="s">
         <v>189</v>
@@ -40741,7 +40740,7 @@
         <v>14</v>
       </c>
       <c r="G144" s="7" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="H144" s="6" t="s">
         <v>1361</v>
@@ -40764,7 +40763,7 @@
         <v>44260</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="D145" s="6" t="s">
         <v>174</v>
@@ -40846,7 +40845,7 @@
         <v>14</v>
       </c>
       <c r="G147" s="7" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="H147" s="6" t="s">
         <v>1361</v>
@@ -40881,7 +40880,7 @@
         <v>14</v>
       </c>
       <c r="G148" s="7" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="H148" s="6" t="s">
         <v>1361</v>
@@ -40916,7 +40915,7 @@
         <v>14</v>
       </c>
       <c r="G149" s="7" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="H149" s="6" t="s">
         <v>1361</v>
@@ -40945,13 +40944,13 @@
         <v>520</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="F150" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G150" s="7" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="H150" s="6" t="s">
         <v>1361</v>
@@ -40974,7 +40973,7 @@
         <v>44260</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="D151" s="6" t="s">
         <v>85</v>
@@ -40986,7 +40985,7 @@
         <v>14</v>
       </c>
       <c r="G151" s="7" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="H151" s="6" t="s">
         <v>1361</v>
@@ -41021,7 +41020,7 @@
         <v>14</v>
       </c>
       <c r="G152" s="7" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="H152" s="6" t="s">
         <v>1361</v>
@@ -41056,7 +41055,7 @@
         <v>14</v>
       </c>
       <c r="G153" s="7" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="H153" s="6" t="s">
         <v>1361</v>
@@ -41079,10 +41078,10 @@
         <v>44260</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="E154" s="6" t="s">
         <v>38</v>
@@ -41120,13 +41119,13 @@
         <v>371</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="F155" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G155" s="7" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="H155" s="6" t="s">
         <v>1361</v>
@@ -41152,7 +41151,7 @@
         <v>803</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="E156" s="6" t="s">
         <v>57</v>
@@ -41161,7 +41160,7 @@
         <v>14</v>
       </c>
       <c r="G156" s="7" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="H156" s="6" t="s">
         <v>1361</v>
@@ -41196,7 +41195,7 @@
         <v>14</v>
       </c>
       <c r="G157" s="7" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="H157" s="6" t="s">
         <v>1361</v>
@@ -41266,7 +41265,7 @@
         <v>14</v>
       </c>
       <c r="G159" s="7" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="H159" s="6" t="s">
         <v>1361</v>
@@ -41324,7 +41323,7 @@
         <v>44260</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="D161" s="6" t="s">
         <v>1102</v>
@@ -41362,7 +41361,7 @@
         <v>660</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="E162" s="6" t="s">
         <v>42</v>
@@ -41394,7 +41393,7 @@
         <v>44260</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="D163" s="6" t="s">
         <v>318</v>
@@ -41406,7 +41405,7 @@
         <v>14</v>
       </c>
       <c r="G163" s="7" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="H163" s="6" t="s">
         <v>1361</v>
@@ -41467,7 +41466,7 @@
         <v>476</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="E165" s="6" t="s">
         <v>42</v>
@@ -41476,7 +41475,7 @@
         <v>14</v>
       </c>
       <c r="G165" s="7" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="H165" s="6" t="s">
         <v>1361</v>
@@ -41537,7 +41536,7 @@
         <v>922</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="E167" s="6" t="s">
         <v>106</v>
@@ -41546,7 +41545,7 @@
         <v>14</v>
       </c>
       <c r="G167" s="7" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="H167" s="6" t="s">
         <v>1361</v>
@@ -41581,7 +41580,7 @@
         <v>14</v>
       </c>
       <c r="G168" s="7" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="H168" s="6" t="s">
         <v>1361</v>
@@ -41607,7 +41606,7 @@
         <v>663</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="E169" s="6" t="s">
         <v>27</v>
@@ -41651,7 +41650,7 @@
         <v>14</v>
       </c>
       <c r="G170" s="7" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="H170" s="6" t="s">
         <v>1361</v>
@@ -41709,10 +41708,10 @@
         <v>44260</v>
       </c>
       <c r="C172" s="6" t="s">
+        <v>1526</v>
+      </c>
+      <c r="D172" s="6" t="s">
         <v>1527</v>
-      </c>
-      <c r="D172" s="6" t="s">
-        <v>1528</v>
       </c>
       <c r="E172" s="6" t="s">
         <v>27</v>
@@ -41744,7 +41743,7 @@
         <v>44260</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="D173" s="6" t="s">
         <v>461</v>
@@ -41791,7 +41790,7 @@
         <v>14</v>
       </c>
       <c r="G174" s="7" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="H174" s="6" t="s">
         <v>16</v>
@@ -41820,13 +41819,13 @@
         <v>138</v>
       </c>
       <c r="E175" s="6" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="F175" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G175" s="7" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="H175" s="6" t="s">
         <v>1361</v>
@@ -41861,7 +41860,7 @@
         <v>14</v>
       </c>
       <c r="G176" s="7" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="H176" s="6" t="s">
         <v>29</v>
@@ -41884,7 +41883,7 @@
         <v>44261</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="D177" s="6" t="s">
         <v>215</v>
@@ -41919,10 +41918,10 @@
         <v>44261</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="D178" s="6" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="E178" s="6" t="s">
         <v>80</v>
@@ -42027,7 +42026,7 @@
         <v>228</v>
       </c>
       <c r="D181" s="6" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="E181" s="6" t="s">
         <v>44</v>
@@ -42374,7 +42373,7 @@
         <v>44261</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="D191" s="5" t="s">
         <v>220</v>
@@ -42409,7 +42408,7 @@
         <v>44261</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="D192" s="5" t="s">
         <v>621</v>
@@ -42421,7 +42420,7 @@
         <v>14</v>
       </c>
       <c r="G192" s="7" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="H192" s="6" t="s">
         <v>1361</v>
@@ -42444,7 +42443,7 @@
         <v>44261</v>
       </c>
       <c r="C193" s="5" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="D193" s="5" t="s">
         <v>921</v>
@@ -42517,7 +42516,7 @@
         <v>784</v>
       </c>
       <c r="D195" s="5" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="E195" s="5" t="s">
         <v>80</v>
@@ -42526,7 +42525,7 @@
         <v>14</v>
       </c>
       <c r="G195" s="7" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="H195" s="6" t="s">
         <v>1361</v>
@@ -42549,10 +42548,10 @@
         <v>44261</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="D196" s="5" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="E196" s="5" t="s">
         <v>27</v>
@@ -42587,7 +42586,7 @@
         <v>789</v>
       </c>
       <c r="D197" s="5" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="E197" s="5" t="s">
         <v>32</v>
@@ -42596,7 +42595,7 @@
         <v>14</v>
       </c>
       <c r="G197" s="7" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="H197" s="6" t="s">
         <v>1361</v>
@@ -42631,10 +42630,10 @@
         <v>14</v>
       </c>
       <c r="G198" s="7" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="H198" s="6" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="I198" s="3" t="s">
         <v>17</v>
@@ -42666,7 +42665,7 @@
         <v>14</v>
       </c>
       <c r="G199" s="7" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="H199" s="6" t="s">
         <v>235</v>
@@ -42689,7 +42688,7 @@
         <v>44262</v>
       </c>
       <c r="C200" s="5" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="D200" s="5" t="s">
         <v>442</v>
@@ -42701,10 +42700,10 @@
         <v>14</v>
       </c>
       <c r="G200" s="7" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="H200" s="6" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="I200" s="3" t="s">
         <v>17</v>
@@ -42730,13 +42729,13 @@
         <v>363</v>
       </c>
       <c r="E201" s="5" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="F201" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G201" s="7" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="H201" s="6" t="s">
         <v>1361</v>
@@ -42771,7 +42770,7 @@
         <v>14</v>
       </c>
       <c r="G202" s="7" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="H202" s="6" t="s">
         <v>1361</v>
@@ -42806,7 +42805,7 @@
         <v>14</v>
       </c>
       <c r="G203" s="7" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="H203" s="6" t="s">
         <v>1361</v>
@@ -42832,7 +42831,7 @@
         <v>618</v>
       </c>
       <c r="D204" s="5" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="E204" s="5" t="s">
         <v>59</v>
@@ -42867,7 +42866,7 @@
         <v>646</v>
       </c>
       <c r="D205" s="5" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="E205" s="5" t="s">
         <v>44</v>
@@ -42876,7 +42875,7 @@
         <v>14</v>
       </c>
       <c r="G205" s="7" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="H205" s="6" t="s">
         <v>1361</v>
@@ -42902,7 +42901,7 @@
         <v>914</v>
       </c>
       <c r="D206" s="5" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="E206" s="5" t="s">
         <v>27</v>
@@ -42934,10 +42933,10 @@
         <v>44262</v>
       </c>
       <c r="C207" s="12" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="D207" s="5" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="E207" s="5" t="s">
         <v>13</v>
@@ -42946,7 +42945,7 @@
         <v>14</v>
       </c>
       <c r="G207" s="11" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="H207" s="6" t="s">
         <v>1361</v>
@@ -42981,7 +42980,7 @@
         <v>14</v>
       </c>
       <c r="G208" s="11" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="H208" s="6" t="s">
         <v>1361</v>
@@ -43004,7 +43003,7 @@
         <v>44262</v>
       </c>
       <c r="C209" s="12" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="D209" s="5" t="s">
         <v>1343</v>
@@ -43042,7 +43041,7 @@
         <v>322</v>
       </c>
       <c r="D210" s="33" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="E210" s="33" t="s">
         <v>32</v>
@@ -43051,7 +43050,7 @@
         <v>14</v>
       </c>
       <c r="G210" s="58" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="H210" s="34" t="s">
         <v>1361</v>
@@ -43086,7 +43085,7 @@
         <v>14</v>
       </c>
       <c r="G211" s="7" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="H211" s="6" t="s">
         <v>1361</v>
@@ -43109,7 +43108,7 @@
         <v>44263</v>
       </c>
       <c r="C212" s="5" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="D212" s="5" t="s">
         <v>1084</v>
@@ -43121,7 +43120,7 @@
         <v>14</v>
       </c>
       <c r="G212" s="7" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="H212" s="6" t="s">
         <v>235</v>
@@ -43144,10 +43143,10 @@
         <v>44263</v>
       </c>
       <c r="C213" s="5" t="s">
+        <v>1575</v>
+      </c>
+      <c r="D213" s="5" t="s">
         <v>1576</v>
-      </c>
-      <c r="D213" s="5" t="s">
-        <v>1577</v>
       </c>
       <c r="E213" s="5" t="s">
         <v>1074</v>
@@ -43156,10 +43155,10 @@
         <v>14</v>
       </c>
       <c r="G213" s="7" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="H213" s="6" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="I213" s="3" t="s">
         <v>17</v>
@@ -43179,10 +43178,10 @@
         <v>44263</v>
       </c>
       <c r="C214" s="5" t="s">
+        <v>1578</v>
+      </c>
+      <c r="D214" s="5" t="s">
         <v>1579</v>
-      </c>
-      <c r="D214" s="5" t="s">
-        <v>1580</v>
       </c>
       <c r="E214" s="5" t="s">
         <v>57</v>
@@ -43191,7 +43190,7 @@
         <v>14</v>
       </c>
       <c r="G214" s="11" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="H214" s="6" t="s">
         <v>1361</v>
@@ -43217,7 +43216,7 @@
         <v>215</v>
       </c>
       <c r="D215" s="5" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="E215" s="5" t="s">
         <v>312</v>
@@ -43226,7 +43225,7 @@
         <v>14</v>
       </c>
       <c r="G215" s="11" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="H215" s="6" t="s">
         <v>1361</v>
@@ -43261,7 +43260,7 @@
         <v>14</v>
       </c>
       <c r="G216" s="11" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="H216" s="6" t="s">
         <v>1361</v>
@@ -43287,7 +43286,7 @@
         <v>1087</v>
       </c>
       <c r="D217" s="5" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="E217" s="5" t="s">
         <v>32</v>
@@ -43296,7 +43295,7 @@
         <v>14</v>
       </c>
       <c r="G217" s="11" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="H217" s="6" t="s">
         <v>1361</v>
@@ -43357,7 +43356,7 @@
         <v>605</v>
       </c>
       <c r="D219" s="5" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="E219" s="5" t="s">
         <v>32</v>
@@ -43392,7 +43391,7 @@
         <v>829</v>
       </c>
       <c r="D220" s="5" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="E220" s="5" t="s">
         <v>38</v>
@@ -43401,10 +43400,10 @@
         <v>14</v>
       </c>
       <c r="G220" s="7" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="H220" s="6" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="I220" s="3" t="s">
         <v>17</v>
@@ -43424,10 +43423,10 @@
         <v>44263</v>
       </c>
       <c r="C221" s="12" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="D221" s="12" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="E221" s="5" t="s">
         <v>57</v>
@@ -43436,7 +43435,7 @@
         <v>14</v>
       </c>
       <c r="G221" s="11" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="H221" s="6" t="s">
         <v>1361</v>
@@ -43471,7 +43470,7 @@
         <v>14</v>
       </c>
       <c r="G222" s="11" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="H222" s="6" t="s">
         <v>1361</v>
@@ -43532,7 +43531,7 @@
         <v>552</v>
       </c>
       <c r="D224" s="5" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="E224" s="5" t="s">
         <v>717</v>
@@ -43541,7 +43540,7 @@
         <v>14</v>
       </c>
       <c r="G224" s="11" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="H224" s="6" t="s">
         <v>1361</v>
@@ -43564,7 +43563,7 @@
         <v>44263</v>
       </c>
       <c r="C225" s="5" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="D225" s="5" t="s">
         <v>520</v>
@@ -43576,7 +43575,7 @@
         <v>14</v>
       </c>
       <c r="G225" s="11" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="H225" s="6" t="s">
         <v>1361</v>
@@ -43602,7 +43601,7 @@
         <v>520</v>
       </c>
       <c r="D226" s="5" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="E226" s="5" t="s">
         <v>267</v>
@@ -43611,7 +43610,7 @@
         <v>14</v>
       </c>
       <c r="G226" s="11" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="H226" s="6" t="s">
         <v>1361</v>
@@ -43646,7 +43645,7 @@
         <v>14</v>
       </c>
       <c r="G227" s="11" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="H227" s="6" t="s">
         <v>1361</v>
@@ -43669,7 +43668,7 @@
         <v>44263</v>
       </c>
       <c r="C228" s="5" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="D228" s="5" t="s">
         <v>521</v>
@@ -43681,7 +43680,7 @@
         <v>14</v>
       </c>
       <c r="G228" s="11" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="H228" s="6" t="s">
         <v>1361</v>
@@ -43707,7 +43706,7 @@
         <v>1033</v>
       </c>
       <c r="D229" s="5" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="E229" s="5" t="s">
         <v>165</v>
@@ -43716,7 +43715,7 @@
         <v>14</v>
       </c>
       <c r="G229" s="11" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="H229" s="6" t="s">
         <v>1361</v>
@@ -43742,7 +43741,7 @@
         <v>1369</v>
       </c>
       <c r="D230" s="5" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="E230" s="5" t="s">
         <v>130</v>
@@ -43751,7 +43750,7 @@
         <v>14</v>
       </c>
       <c r="G230" s="11" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="H230" s="6" t="s">
         <v>1361</v>
@@ -43786,7 +43785,7 @@
         <v>14</v>
       </c>
       <c r="G231" s="11" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="H231" s="6" t="s">
         <v>1361</v>
@@ -43812,7 +43811,7 @@
         <v>1270</v>
       </c>
       <c r="D232" s="5" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="E232" s="5" t="s">
         <v>685</v>
@@ -43821,7 +43820,7 @@
         <v>14</v>
       </c>
       <c r="G232" s="11" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="H232" s="6" t="s">
         <v>1361</v>
@@ -43856,7 +43855,7 @@
         <v>14</v>
       </c>
       <c r="G233" s="11" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="H233" s="6" t="s">
         <v>1361</v>
@@ -43882,7 +43881,7 @@
         <v>711</v>
       </c>
       <c r="D234" s="5" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="E234" s="5" t="s">
         <v>195</v>
@@ -43891,7 +43890,7 @@
         <v>14</v>
       </c>
       <c r="G234" s="11" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="H234" s="6" t="s">
         <v>1361</v>
@@ -43926,7 +43925,7 @@
         <v>14</v>
       </c>
       <c r="G235" s="11" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="H235" s="6" t="s">
         <v>1361</v>
@@ -43961,7 +43960,7 @@
         <v>14</v>
       </c>
       <c r="G236" s="11" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="H236" s="6" t="s">
         <v>1361</v>
@@ -43990,13 +43989,13 @@
         <v>1226</v>
       </c>
       <c r="E237" s="5" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="F237" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G237" s="11" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="H237" s="6" t="s">
         <v>1361</v>
@@ -44022,7 +44021,7 @@
         <v>396</v>
       </c>
       <c r="D238" s="5" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="E238" s="5" t="s">
         <v>312</v>
@@ -44031,7 +44030,7 @@
         <v>14</v>
       </c>
       <c r="G238" s="11" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="H238" s="6" t="s">
         <v>1361</v>
@@ -44066,7 +44065,7 @@
         <v>14</v>
       </c>
       <c r="G239" s="11" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="H239" s="6" t="s">
         <v>1361</v>
@@ -44092,7 +44091,7 @@
         <v>915</v>
       </c>
       <c r="D240" s="5" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="E240" s="5" t="s">
         <v>165</v>
@@ -44101,7 +44100,7 @@
         <v>14</v>
       </c>
       <c r="G240" s="11" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="H240" s="6" t="s">
         <v>1361</v>
@@ -44127,7 +44126,7 @@
         <v>1103</v>
       </c>
       <c r="D241" s="5" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="E241" s="5" t="s">
         <v>53</v>
@@ -44136,7 +44135,7 @@
         <v>14</v>
       </c>
       <c r="G241" s="11" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="H241" s="6" t="s">
         <v>1361</v>
@@ -44229,10 +44228,10 @@
         <v>44263</v>
       </c>
       <c r="C244" s="5" t="s">
+        <v>1603</v>
+      </c>
+      <c r="D244" s="5" t="s">
         <v>1604</v>
-      </c>
-      <c r="D244" s="5" t="s">
-        <v>1605</v>
       </c>
       <c r="E244" s="5" t="s">
         <v>27</v>
@@ -44264,7 +44263,7 @@
         <v>44263</v>
       </c>
       <c r="C245" s="5" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="D245" s="5" t="s">
         <v>314</v>
@@ -44299,10 +44298,10 @@
         <v>44263</v>
       </c>
       <c r="C246" s="5" t="s">
+        <v>1605</v>
+      </c>
+      <c r="D246" s="5" t="s">
         <v>1606</v>
-      </c>
-      <c r="D246" s="5" t="s">
-        <v>1607</v>
       </c>
       <c r="E246" s="5" t="s">
         <v>44</v>
@@ -44334,10 +44333,10 @@
         <v>44263</v>
       </c>
       <c r="C247" s="5" t="s">
+        <v>1607</v>
+      </c>
+      <c r="D247" s="5" t="s">
         <v>1608</v>
-      </c>
-      <c r="D247" s="5" t="s">
-        <v>1609</v>
       </c>
       <c r="E247" s="5" t="s">
         <v>27</v>
@@ -44372,7 +44371,7 @@
         <v>1188</v>
       </c>
       <c r="D248" s="5" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="E248" s="5" t="s">
         <v>106</v>
@@ -44416,7 +44415,7 @@
         <v>14</v>
       </c>
       <c r="G249" s="11" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="H249" s="6" t="s">
         <v>1361</v>
@@ -44451,7 +44450,7 @@
         <v>14</v>
       </c>
       <c r="G250" s="11" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="H250" s="6" t="s">
         <v>1361</v>
@@ -44477,7 +44476,7 @@
         <v>1079</v>
       </c>
       <c r="D251" s="5" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="E251" s="5" t="s">
         <v>369</v>
@@ -44486,7 +44485,7 @@
         <v>14</v>
       </c>
       <c r="G251" s="7" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="H251" s="6" t="s">
         <v>1361</v>
@@ -44547,7 +44546,7 @@
         <v>536</v>
       </c>
       <c r="D253" s="5" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="E253" s="5" t="s">
         <v>53</v>
@@ -44556,7 +44555,7 @@
         <v>14</v>
       </c>
       <c r="G253" s="11" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="H253" s="6" t="s">
         <v>1361</v>
@@ -44591,10 +44590,10 @@
         <v>14</v>
       </c>
       <c r="G254" s="11" t="s">
+        <v>1614</v>
+      </c>
+      <c r="H254" s="6" t="s">
         <v>1615</v>
-      </c>
-      <c r="H254" s="6" t="s">
-        <v>1616</v>
       </c>
       <c r="I254" s="3" t="s">
         <v>17</v>
@@ -44617,7 +44616,7 @@
         <v>789</v>
       </c>
       <c r="D255" s="5" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="E255" s="5" t="s">
         <v>44</v>
@@ -44661,7 +44660,7 @@
         <v>14</v>
       </c>
       <c r="G256" s="11" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="H256" s="6" t="s">
         <v>1361</v>
@@ -44696,7 +44695,7 @@
         <v>14</v>
       </c>
       <c r="G257" s="7" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="H257" s="6" t="s">
         <v>16</v>
@@ -44766,7 +44765,7 @@
         <v>14</v>
       </c>
       <c r="G259" s="11" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="H259" s="6" t="s">
         <v>70</v>
@@ -44789,7 +44788,7 @@
         <v>44264</v>
       </c>
       <c r="C260" s="5" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="D260" s="5" t="s">
         <v>629</v>
@@ -44801,7 +44800,7 @@
         <v>14</v>
       </c>
       <c r="G260" s="11" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="H260" s="6" t="s">
         <v>70</v>
@@ -44827,7 +44826,7 @@
         <v>1401</v>
       </c>
       <c r="D261" s="5" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="E261" s="5" t="s">
         <v>13</v>
@@ -44836,7 +44835,7 @@
         <v>14</v>
       </c>
       <c r="G261" s="11" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="H261" s="6" t="s">
         <v>70</v>
@@ -44859,7 +44858,7 @@
         <v>44264</v>
       </c>
       <c r="C262" s="5" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="D262" s="5" t="s">
         <v>154</v>
@@ -44871,7 +44870,7 @@
         <v>14</v>
       </c>
       <c r="G262" s="11" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="H262" s="6" t="s">
         <v>70</v>
@@ -44906,10 +44905,10 @@
         <v>14</v>
       </c>
       <c r="G263" s="7" t="s">
+        <v>1626</v>
+      </c>
+      <c r="H263" s="6" t="s">
         <v>1627</v>
-      </c>
-      <c r="H263" s="6" t="s">
-        <v>1628</v>
       </c>
       <c r="I263" s="3" t="s">
         <v>17</v>
@@ -44941,7 +44940,7 @@
         <v>14</v>
       </c>
       <c r="G264" s="11" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="H264" s="6" t="s">
         <v>1361</v>
@@ -44964,10 +44963,10 @@
         <v>44264</v>
       </c>
       <c r="C265" s="5" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="D265" s="5" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="E265" s="5" t="s">
         <v>165</v>
@@ -44976,7 +44975,7 @@
         <v>14</v>
       </c>
       <c r="G265" s="11" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="H265" s="6" t="s">
         <v>1361</v>
@@ -45011,7 +45010,7 @@
         <v>14</v>
       </c>
       <c r="G266" s="11" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="H266" s="6" t="s">
         <v>1361</v>
@@ -45046,7 +45045,7 @@
         <v>14</v>
       </c>
       <c r="G267" s="11" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="H267" s="6" t="s">
         <v>1361</v>
@@ -45081,7 +45080,7 @@
         <v>14</v>
       </c>
       <c r="G268" s="11" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="H268" s="6" t="s">
         <v>1361</v>
@@ -45104,7 +45103,7 @@
         <v>44264</v>
       </c>
       <c r="C269" s="5" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="D269" s="5" t="s">
         <v>469</v>
@@ -45151,7 +45150,7 @@
         <v>14</v>
       </c>
       <c r="G270" s="11" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="H270" s="6" t="s">
         <v>1361</v>
@@ -45177,7 +45176,7 @@
         <v>692</v>
       </c>
       <c r="D271" s="5" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="E271" s="5" t="s">
         <v>13</v>
@@ -45244,7 +45243,7 @@
         <v>44264</v>
       </c>
       <c r="C273" s="5" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="D273" s="5" t="s">
         <v>83</v>
@@ -45291,7 +45290,7 @@
         <v>14</v>
       </c>
       <c r="G274" s="11" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="H274" s="6" t="s">
         <v>1361</v>
@@ -45326,7 +45325,7 @@
         <v>14</v>
       </c>
       <c r="G275" s="11" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="H275" s="6" t="s">
         <v>1361</v>
@@ -45419,7 +45418,7 @@
         <v>44264</v>
       </c>
       <c r="C278" s="5" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="D278" s="5" t="s">
         <v>640</v>
@@ -45431,7 +45430,7 @@
         <v>14</v>
       </c>
       <c r="G278" s="11" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="H278" s="6" t="s">
         <v>1361</v>
@@ -45454,7 +45453,7 @@
         <v>44264</v>
       </c>
       <c r="C279" s="5" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="D279" s="5" t="s">
         <v>1428</v>
@@ -45466,7 +45465,7 @@
         <v>14</v>
       </c>
       <c r="G279" s="11" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="H279" s="6" t="s">
         <v>1361</v>
@@ -45489,7 +45488,7 @@
         <v>44264</v>
       </c>
       <c r="C280" s="5" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="D280" s="5" t="s">
         <v>1002</v>
@@ -45501,7 +45500,7 @@
         <v>14</v>
       </c>
       <c r="G280" s="11" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="H280" s="6" t="s">
         <v>1361</v>
@@ -45536,7 +45535,7 @@
         <v>14</v>
       </c>
       <c r="G281" s="11" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="H281" s="6" t="s">
         <v>1361</v>
@@ -45559,7 +45558,7 @@
         <v>44264</v>
       </c>
       <c r="C282" s="5" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="D282" s="5" t="s">
         <v>805</v>
@@ -45571,7 +45570,7 @@
         <v>14</v>
       </c>
       <c r="G282" s="11" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="H282" s="6" t="s">
         <v>1361</v>
@@ -45606,7 +45605,7 @@
         <v>14</v>
       </c>
       <c r="G283" s="11" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="H283" s="6" t="s">
         <v>1361</v>
@@ -45629,10 +45628,10 @@
         <v>44264</v>
       </c>
       <c r="C284" s="5" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D284" s="5" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="E284" s="5" t="s">
         <v>369</v>
@@ -45641,7 +45640,7 @@
         <v>14</v>
       </c>
       <c r="G284" s="11" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="H284" s="6" t="s">
         <v>1361</v>
@@ -45667,7 +45666,7 @@
         <v>194</v>
       </c>
       <c r="D285" s="5" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="E285" s="5" t="s">
         <v>59</v>
@@ -45679,7 +45678,7 @@
         <v>1357</v>
       </c>
       <c r="H285" s="6" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="I285" s="3" t="s">
         <v>17</v>
@@ -45699,7 +45698,7 @@
         <v>44264</v>
       </c>
       <c r="C286" s="5" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="D286" s="5" t="s">
         <v>1287</v>
@@ -45711,7 +45710,7 @@
         <v>14</v>
       </c>
       <c r="G286" s="11" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="H286" s="6" t="s">
         <v>1361</v>
@@ -45737,7 +45736,7 @@
         <v>1287</v>
       </c>
       <c r="D287" s="12" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="E287" s="5" t="s">
         <v>27</v>
@@ -45746,7 +45745,7 @@
         <v>14</v>
       </c>
       <c r="G287" s="11" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="H287" s="6" t="s">
         <v>1361</v>
@@ -45769,7 +45768,7 @@
         <v>44264</v>
       </c>
       <c r="C288" s="5" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D288" s="5" t="s">
         <v>231</v>
@@ -45781,7 +45780,7 @@
         <v>14</v>
       </c>
       <c r="G288" s="11" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="H288" s="6" t="s">
         <v>1361</v>
@@ -45851,7 +45850,7 @@
         <v>14</v>
       </c>
       <c r="G290" s="11" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="H290" s="6" t="s">
         <v>1361</v>
@@ -45874,7 +45873,7 @@
         <v>44264</v>
       </c>
       <c r="C291" s="5" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="D291" s="5" t="s">
         <v>1436</v>
@@ -45912,7 +45911,7 @@
         <v>915</v>
       </c>
       <c r="D292" s="5" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="E292" s="5" t="s">
         <v>27</v>
@@ -45921,7 +45920,7 @@
         <v>14</v>
       </c>
       <c r="G292" s="11" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="H292" s="6" t="s">
         <v>1361</v>
@@ -45944,10 +45943,10 @@
         <v>44264</v>
       </c>
       <c r="C293" s="5" t="s">
+        <v>1649</v>
+      </c>
+      <c r="D293" s="5" t="s">
         <v>1650</v>
-      </c>
-      <c r="D293" s="5" t="s">
-        <v>1651</v>
       </c>
       <c r="E293" s="5" t="s">
         <v>27</v>
@@ -46016,8 +46015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView topLeftCell="C52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -46779,7 +46778,7 @@
         <v>44258</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>325</v>
@@ -46791,7 +46790,7 @@
         <v>14</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>29</v>
@@ -46876,7 +46875,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="96" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -46896,7 +46895,7 @@
         <v>14</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>1447</v>
+        <v>1651</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>235</v>
@@ -46919,10 +46918,10 @@
         <v>44259</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>1449</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>1450</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>80</v>
@@ -46954,10 +46953,10 @@
         <v>44259</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>1451</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>1452</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>42</v>
@@ -46989,7 +46988,7 @@
         <v>44259</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>1322</v>
@@ -47001,7 +47000,7 @@
         <v>14</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>70</v>
@@ -47036,10 +47035,10 @@
         <v>14</v>
       </c>
       <c r="G29" s="7" t="s">
+        <v>1465</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>1466</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>1467</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>17</v>
@@ -47071,10 +47070,10 @@
         <v>14</v>
       </c>
       <c r="G30" s="7" t="s">
+        <v>1465</v>
+      </c>
+      <c r="H30" s="5" t="s">
         <v>1466</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>1467</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>17</v>
@@ -47094,7 +47093,7 @@
         <v>44259</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>1296</v>
@@ -47106,7 +47105,7 @@
         <v>14</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>235</v>
@@ -47132,7 +47131,7 @@
         <v>1260</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>189</v>
@@ -47141,7 +47140,7 @@
         <v>14</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>235</v>
@@ -47202,7 +47201,7 @@
         <v>413</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>53</v>
@@ -47211,7 +47210,7 @@
         <v>14</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>235</v>
@@ -47246,7 +47245,7 @@
         <v>14</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>70</v>
@@ -47269,10 +47268,10 @@
         <v>44260</v>
       </c>
       <c r="C36" s="5" t="s">
+        <v>1487</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>1488</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>1489</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>80</v>
@@ -47304,10 +47303,10 @@
         <v>44260</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>1496</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>1497</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>27</v>
@@ -47316,7 +47315,7 @@
         <v>14</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>235</v>
@@ -47351,7 +47350,7 @@
         <v>14</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>235</v>
@@ -47375,7 +47374,7 @@
         <v>724</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>32</v>
@@ -47404,7 +47403,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>1204</v>
@@ -47413,13 +47412,13 @@
         <v>987</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>14</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>235</v>
@@ -47442,10 +47441,10 @@
         <v>44260</v>
       </c>
       <c r="C41" s="12" t="s">
+        <v>1530</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>1531</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>1532</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>44</v>
@@ -47454,7 +47453,7 @@
         <v>14</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>235</v>
@@ -47489,7 +47488,7 @@
         <v>14</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>16</v>
@@ -47515,7 +47514,7 @@
         <v>126</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>717</v>
@@ -47524,7 +47523,7 @@
         <v>14</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>235</v>
@@ -47550,7 +47549,7 @@
         <v>793</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>44</v>
@@ -47559,7 +47558,7 @@
         <v>14</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>235</v>
@@ -47585,7 +47584,7 @@
         <v>160</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>80</v>
@@ -47664,7 +47663,7 @@
         <v>14</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>235</v>
@@ -47724,7 +47723,7 @@
         <v>14</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>235</v>
@@ -47759,7 +47758,7 @@
         <v>14</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>235</v>
@@ -47794,7 +47793,7 @@
         <v>14</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>235</v>
@@ -47899,10 +47898,10 @@
         <v>14</v>
       </c>
       <c r="G54" s="11" t="s">
+        <v>1614</v>
+      </c>
+      <c r="H54" s="6" t="s">
         <v>1615</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>1616</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>17</v>
@@ -47934,7 +47933,7 @@
         <v>14</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>16</v>
@@ -47969,7 +47968,7 @@
         <v>14</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>16</v>
@@ -48004,7 +48003,7 @@
         <v>14</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>235</v>
@@ -48039,7 +48038,7 @@
         <v>14</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>70</v>
@@ -48065,7 +48064,7 @@
         <v>630</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>80</v>
@@ -48074,7 +48073,7 @@
         <v>14</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>235</v>
@@ -48100,7 +48099,7 @@
         <v>793</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>44</v>
@@ -48109,7 +48108,7 @@
         <v>14</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>235</v>
@@ -48144,7 +48143,7 @@
         <v>14</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>235</v>
@@ -48179,7 +48178,7 @@
         <v>14</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>235</v>
@@ -48205,7 +48204,7 @@
         <v>704</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>80</v>
@@ -48214,7 +48213,7 @@
         <v>14</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="H63" s="6" t="s">
         <v>70</v>
@@ -48240,7 +48239,7 @@
         <v>194</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>59</v>
@@ -48249,7 +48248,7 @@
         <v>14</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="H64" s="6" t="s">
         <v>235</v>

</xml_diff>